<commit_message>
added Form 2400 valuesets from Symedical
</commit_message>
<xml_diff>
--- a/docs/ValueSet-med-all-form2400-vs.xlsx
+++ b/docs/ValueSet-med-all-form2400-vs.xlsx
@@ -13,21 +13,12 @@
     <sheet name="Include ValueSets 4" r:id="rId7" sheetId="5"/>
     <sheet name="Include ValueSets 5" r:id="rId8" sheetId="6"/>
     <sheet name="Include ValueSets 6" r:id="rId9" sheetId="7"/>
-    <sheet name="Include ValueSets 7" r:id="rId10" sheetId="8"/>
-    <sheet name="Include ValueSets 8" r:id="rId11" sheetId="9"/>
-    <sheet name="Include ValueSets 9" r:id="rId12" sheetId="10"/>
-    <sheet name="Include ValueSets 10" r:id="rId13" sheetId="11"/>
-    <sheet name="Include ValueSets 11" r:id="rId14" sheetId="12"/>
-    <sheet name="Include ValueSets 12" r:id="rId15" sheetId="13"/>
-    <sheet name="Include ValueSets 13" r:id="rId16" sheetId="14"/>
-    <sheet name="Include ValueSets 14" r:id="rId17" sheetId="15"/>
-    <sheet name="Include ValueSets 15" r:id="rId18" sheetId="16"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Property</t>
   </si>
@@ -71,7 +62,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-08-02T15:12:35-05:00</t>
+    <t>2022-08-09T16:48:03-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -107,49 +98,22 @@
     <t>ValueSet URL</t>
   </si>
   <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-alemtuzumab-vs</t>
-  </si>
-  <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-anti-thymocyte-globulin-vs</t>
-  </si>
-  <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-bortezomib-vs</t>
-  </si>
-  <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-busulfan-vs</t>
-  </si>
-  <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-carmustine-vs</t>
-  </si>
-  <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-cyclophosphamide-vs</t>
-  </si>
-  <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-cytarabine-vs</t>
-  </si>
-  <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-defibrotide-vs</t>
-  </si>
-  <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-etoposide-vs</t>
-  </si>
-  <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-fludarabine-vs</t>
-  </si>
-  <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-melphalan-vs</t>
-  </si>
-  <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-rituximab-vs</t>
-  </si>
-  <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-thiotepa-vs</t>
-  </si>
-  <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-treosulfan-vs</t>
-  </si>
-  <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-ursodiol-vs</t>
+    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-addition-peri-transplant-vs</t>
+  </si>
+  <si>
+    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-gvhd-prophylaxis-vs</t>
+  </si>
+  <si>
+    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-mobilizing-agents-vs</t>
+  </si>
+  <si>
+    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-post-hct-disease-therapy-planned-vs</t>
+  </si>
+  <si>
+    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-prep-regiment-vs</t>
+  </si>
+  <si>
+    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/med-prior-exposure-vs</t>
   </si>
 </sst>
 </file>
@@ -412,7 +376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -431,15 +395,15 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -458,15 +422,15 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -485,15 +449,15 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -512,15 +476,15 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -539,15 +503,15 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -566,253 +530,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="30.703125" customWidth="true"/>
-    <col min="2" max="2" width="50.703125" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="30.703125" customWidth="true"/>
-    <col min="2" max="2" width="50.703125" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="30.703125" customWidth="true"/>
-    <col min="2" max="2" width="50.703125" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="30.703125" customWidth="true"/>
-    <col min="2" max="2" width="50.703125" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="30.703125" customWidth="true"/>
-    <col min="2" max="2" width="50.703125" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="30.703125" customWidth="true"/>
-    <col min="2" max="2" width="50.703125" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="30.703125" customWidth="true"/>
-    <col min="2" max="2" width="50.703125" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="30.703125" customWidth="true"/>
-    <col min="2" max="2" width="50.703125" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="30.703125" customWidth="true"/>
-    <col min="2" max="2" width="50.703125" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>